<commit_message>
Business logic to plugins.
- MQTT processing to iotgate.
- SoC temperature measurement to system.
</commit_message>
<xml_diff>
--- a/MQTT_topics.xlsx
+++ b/MQTT_topics.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="36">
   <si>
     <t>Category</t>
   </si>
@@ -110,7 +110,25 @@
     <t>measure</t>
   </si>
   <si>
-    <t>value</t>
+    <t>percon</t>
+  </si>
+  <si>
+    <t>percoff</t>
+  </si>
+  <si>
+    <t>tempon</t>
+  </si>
+  <si>
+    <t>tempoff</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>payload (value)</t>
+  </si>
+  <si>
+    <t>system</t>
   </si>
 </sst>
 </file>
@@ -477,7 +495,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,7 +506,7 @@
     <col min="5" max="5" width="30.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -502,12 +520,15 @@
         <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -522,9 +543,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -539,7 +560,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -556,7 +577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -564,16 +585,14 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -581,16 +600,14 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -598,16 +615,14 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="4">
         <v>71.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -615,16 +630,14 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -641,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -649,16 +662,14 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -666,16 +677,14 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -683,16 +692,14 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="4">
         <v>71.25</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -700,16 +707,14 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added plugins filtering by prefix and plugin development.
</commit_message>
<xml_diff>
--- a/MQTT_topics.xlsx
+++ b/MQTT_topics.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="38">
   <si>
     <t>Category</t>
   </si>
@@ -86,10 +86,6 @@
   </si>
   <si>
     <t>off</t>
-  </si>
-  <si>
-    <t>Toto sú pevné kategórie, ktoré brána rozlišuje. Zodpovedajú vstupným bodom pluginov.
-Poznajú ich len brána a hardvérový komponent. Brána len volá im zodpovedajúce metódy pluginu.</t>
   </si>
   <si>
     <t>Značka zariadenia. Je to názov originálneho hardvérového komponentu, napr. senzora a tento touto značkou uvádza všetky MQTT témy, do ktorých vysiela a prijíma správy.
@@ -128,7 +124,17 @@
     <t>payload (value)</t>
   </si>
   <si>
-    <t>system</t>
+    <t>iotgate</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STATUS, RESET</t>
+  </si>
+  <si>
+    <t>Toto sú pevné vymenované kategórie, ktoré brána rozlišuje pre každy plugin rovnako. Zodpovedajú funkcionalitám pluginov.
+Poznajú ich len brána a hardvérový komponent. Brána len volá im zodpovedajúce metódy pluginu.</t>
   </si>
 </sst>
 </file>
@@ -491,11 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,27 +514,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -545,7 +551,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -553,58 +559,62 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="4">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="E4" s="4">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="4">
-        <v>95</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4">
-        <v>60</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -614,12 +624,14 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="4">
-        <v>71.25</v>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -630,11 +642,11 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4">
-        <v>45</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -642,16 +654,14 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -659,14 +669,14 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="4">
-        <v>85</v>
+        <v>71.25</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -674,14 +684,14 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="4">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -691,12 +701,14 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4">
-        <v>71.25</v>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -707,55 +719,98 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="4">
-        <v>45</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="4">
+        <v>71.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="130.5" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="59.25" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="130.5" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
@@ -769,10 +824,29 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="59.25" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A18:J18"/>
     <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added plugin for ThingSpeak and further plugin development.
</commit_message>
<xml_diff>
--- a/MQTT_topics.xlsx
+++ b/MQTT_topics.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\431938\Documents\My Office Documents\ICC\GitHub\iot\iotgate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979E73A-6CCB-45BB-8F68-E2BD5A5B4A98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sémantické členenie" sheetId="4" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="48">
   <si>
     <t>Category</t>
   </si>
@@ -112,12 +118,6 @@
     <t>percoff</t>
   </si>
   <si>
-    <t>tempon</t>
-  </si>
-  <si>
-    <t>tempoff</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -130,21 +130,86 @@
     <t>period</t>
   </si>
   <si>
-    <t xml:space="preserve"> STATUS, RESET</t>
-  </si>
-  <si>
-    <t>Toto sú pevné vymenované kategórie, ktoré brána rozlišuje pre každy plugin rovnako. Zodpovedajú funkcionalitám pluginov.
-Poznajú ich len brána a hardvérový komponent. Brána len volá im zodpovedajúce metódy pluginu.</t>
+    <t>run</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>PA13</t>
+  </si>
+  <si>
+    <t>enum: Active, Idle, Unknown</t>
+  </si>
+  <si>
+    <t>dft</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>enum: STATUS, RESET, ON, OFF, TOGGLE</t>
+  </si>
+  <si>
+    <t>enum: STATUS, RESET</t>
+  </si>
+  <si>
+    <t>sfan</t>
+  </si>
+  <si>
+    <t>Skratka stavovej veličiny, ktorá je súčasťou charakteristiky stavu zariadenia. Každé zariadenie (plugin) má spravidla osobitný zoznam parametrov, hoci niektoré sú zhodné pre viaceré zariadenia, napríklad perióda opakovania časovača.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Skratka povahy údajovo prenášaných v MQTT správe. Je to vymenovaná množina kategórii spoločná pre všetky zariadenia.
+Použité kategória: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>state, cmd, data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Skratka štatistickej veličiny parametra, ak je parameter povahy fyzikálnej veličiny. Je to vymenovaná množina skratiek spoločná pre všetky zariadenia.
+Použité veličiny: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>val, dft, min, max, avg, ptl, perc</t>
+    </r>
+  </si>
+  <si>
+    <t>Timer period for measuring SoC temperature</t>
+  </si>
+  <si>
+    <t>Timer period for reconnecting MQTT broker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,7 +236,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -179,11 +244,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -195,9 +269,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="normálne" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -213,7 +292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -255,7 +334,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,9 +366,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,6 +418,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,23 +611,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24:J24"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -526,13 +643,13 @@
         <v>27</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -549,7 +666,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -566,7 +683,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -583,270 +700,538 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="8">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="4">
-        <v>71.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E13" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="4">
-        <v>71.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E18" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="2" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="8">
+        <v>70</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="4">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="130.5" customHeight="1">
-      <c r="A21" s="6" t="s">
+    <row r="33" spans="1:10" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="2" t="s">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="59.25" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+    <row r="36" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A24:J24"/>
+  <mergeCells count="4">
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A42:J42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -854,7 +1239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -862,7 +1247,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -872,7 +1257,7 @@
     <col min="6" max="6" width="30.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -892,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -912,7 +1297,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -932,7 +1317,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -952,7 +1337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -972,7 +1357,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -992,7 +1377,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1012,7 +1397,7 @@
         <v>71.25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1032,7 +1417,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1052,7 +1437,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1072,7 +1457,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1092,7 +1477,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1497,7 @@
         <v>71.25</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +1517,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1159,24 +1544,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Plugin updated according to the iot library changes.
</commit_message>
<xml_diff>
--- a/MQTT_topics.xlsx
+++ b/MQTT_topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\431938\Documents\My Office Documents\ICC\GitHub\iot\iotgate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979E73A-6CCB-45BB-8F68-E2BD5A5B4A98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA1A699-828A-42E8-88F2-F199C484BD3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="54">
   <si>
     <t>Category</t>
   </si>
@@ -196,10 +196,28 @@
     </r>
   </si>
   <si>
-    <t>Timer period for measuring SoC temperature</t>
-  </si>
-  <si>
-    <t>Timer period for reconnecting MQTT broker</t>
+    <t>Perióda časovača na meranie systémovej teploty</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Hodnota prenášaná v správach príslušného topiku. Tu je uvedený typický príklad, resp. v kóde zabudované a predvolené hodnoty.</t>
+  </si>
+  <si>
+    <t>Čítané pluginom "sfan" a "thingspeak"</t>
+  </si>
+  <si>
+    <t>Čítané pluginom "thingspeak"</t>
+  </si>
+  <si>
+    <t>Perióda časovača na kontrolu a obnovenie spojenia s MQTT brokerom</t>
+  </si>
+  <si>
+    <t>thinkspeak</t>
+  </si>
+  <si>
+    <t>Perióda časovača na publikovanie načítaných dát do cloudu</t>
   </si>
 </sst>
 </file>
@@ -257,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -266,14 +284,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,21 +636,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -665,6 +689,9 @@
       <c r="E2" s="4">
         <v>60</v>
       </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -682,6 +709,9 @@
       <c r="E3" s="4">
         <v>80</v>
       </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -789,22 +819,22 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>10</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -822,6 +852,9 @@
       <c r="E11" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1011,22 +1044,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>70</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1062,7 +1095,7 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1133,105 +1166,229 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="7">
         <v>60</v>
       </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="4">
+        <v>60</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="4">
+        <v>600</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="7">
+        <v>60</v>
+      </c>
       <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-    </row>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    <row r="45" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="48" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A42:J42"/>
+  <mergeCells count="5">
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A48:F48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Introduced 'blynk' plugin and launching 'run' method from all plugins.
</commit_message>
<xml_diff>
--- a/MQTT_topics.xlsx
+++ b/MQTT_topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\431938\Documents\My Office Documents\ICC\GitHub\iot\iotgate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA1A699-828A-42E8-88F2-F199C484BD3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E03AD1D-B4B5-44E3-B7E7-9026B49958B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="60">
   <si>
     <t>Category</t>
   </si>
@@ -218,6 +218,24 @@
   </si>
   <si>
     <t>Perióda časovača na publikovanie načítaných dát do cloudu</t>
+  </si>
+  <si>
+    <t>blynk</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>cfan</t>
+  </si>
+  <si>
+    <t>Virtuálny pin v mobilnej aplikácii na zobrazenie prijatej SoC teploty</t>
+  </si>
+  <si>
+    <t>Virtuálny pin v mobilnej aplikácii na ovládanie chladiaceho ventilátora</t>
   </si>
 </sst>
 </file>
@@ -290,13 +308,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,11 +654,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,10 +882,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>36</v>
@@ -1290,105 +1308,145 @@
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="41" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+    <row r="44" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+    <row r="47" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="50" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Blynk and Thinkspeak plugin fixed.
</commit_message>
<xml_diff>
--- a/MQTT_topics.xlsx
+++ b/MQTT_topics.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\431938\Documents\My Office Documents\ICC\GitHub\iot\iotgate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E03AD1D-B4B5-44E3-B7E7-9026B49958B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sémantické členenie" sheetId="4" r:id="rId1"/>
@@ -23,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="58">
   <si>
     <t>Category</t>
   </si>
@@ -223,12 +217,6 @@
     <t>blynk</t>
   </si>
   <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>V2</t>
-  </si>
-  <si>
     <t>cfan</t>
   </si>
   <si>
@@ -241,11 +229,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -316,9 +304,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="normálne" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -334,7 +328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -376,7 +370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,27 +402,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,24 +436,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -653,15 +611,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -671,7 +629,7 @@
     <col min="6" max="6" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -691,7 +649,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -711,7 +669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -731,7 +689,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -748,7 +706,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -768,7 +726,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -785,7 +743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -802,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -819,7 +777,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -836,7 +794,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -854,7 +812,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" thickTop="1">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -874,7 +832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -882,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>35</v>
@@ -891,7 +849,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -908,7 +866,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -925,7 +883,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -942,7 +900,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -959,7 +917,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -976,7 +934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -993,7 +951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1010,7 +968,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1027,7 +985,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1044,7 +1002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1061,7 +1019,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
       <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
@@ -1079,7 +1037,7 @@
       </c>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" thickTop="1">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1096,7 +1054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1116,7 +1074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1133,7 +1091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1167,7 +1125,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1184,7 +1142,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
@@ -1202,7 +1160,7 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" thickTop="1">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1222,7 +1180,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -1239,7 +1197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1256,7 +1214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1273,7 +1231,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1290,7 +1248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1">
       <c r="A36" s="6" t="s">
         <v>52</v>
       </c>
@@ -1308,7 +1266,7 @@
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" thickTop="1">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -1321,14 +1279,14 @@
       <c r="D37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>55</v>
+      <c r="E37" s="12">
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
@@ -1336,25 +1294,25 @@
         <v>7</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>56</v>
+      <c r="E38" s="13">
+        <v>3</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="70.5" customHeight="1">
       <c r="A41" s="11" t="s">
         <v>23</v>
       </c>
@@ -1368,12 +1326,12 @@
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="40.5" customHeight="1">
       <c r="A44" s="11" t="s">
         <v>44</v>
       </c>
@@ -1387,12 +1345,12 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="46.5" customHeight="1">
       <c r="A47" s="11" t="s">
         <v>43</v>
       </c>
@@ -1406,12 +1364,12 @@
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="49.5" customHeight="1">
       <c r="A50" s="11" t="s">
         <v>45</v>
       </c>
@@ -1425,12 +1383,12 @@
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="10" t="s">
         <v>48</v>
       </c>
@@ -1454,7 +1412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1462,7 +1420,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -1472,7 +1430,7 @@
     <col min="6" max="6" width="30.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1492,7 +1450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1512,7 +1470,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1532,7 +1490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1552,7 +1510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1572,7 +1530,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1592,7 +1550,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1570,7 @@
         <v>71.25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1590,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1652,7 +1610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1630,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1692,7 +1650,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1712,7 +1670,7 @@
         <v>71.25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1732,7 +1690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1759,24 +1717,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>